<commit_message>
Updated Timesheet - Remuki
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet  1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet  1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3AA990E-86F5-47C9-92AB-36F9FEBD82D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{14F69019-6753-4D0C-9098-ADCDD4704E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
     <sheet name="Day15 ( 23-04-2022 )" sheetId="54" r:id="rId13"/>
     <sheet name="Day16 (25-04-2022) (2)" sheetId="58" r:id="rId14"/>
     <sheet name="Day17(26-04-2022)" sheetId="57" r:id="rId15"/>
-    <sheet name="Day18(27-04-2022) " sheetId="59" r:id="rId16"/>
+    <sheet name="Day18(27-04-2022)  (2)" sheetId="61" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="265">
   <si>
     <t>Column1</t>
   </si>
@@ -1209,6 +1209,14 @@
 3.30pm to 4.00pm : worked on estimations(mapped views with operations for Interviewer, Management and Admin)
 4.30pm to 5.45pm : worked on estimations(mapped views with operations for Admin and refined estimations)
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+8:45 to 9:00       - Checked in the mail.
+9:00 to 9:30       - Working on listing page.
+9:30 to 10:30      - Softskills session with savitha ( Problem solving).
+10:30 to 10:45    - Break
+10:45 to 1:00       - continued on listing (pagination,responsiveness).                                                  1:00 to 1:15          -Idle.                                                            1:15 to 2:00          - Lunch.                                                        2:00 to 2:30          -working on responsiveness for upcoming drives page.                                                             2:30 to 2:50          -Review meeting with Rafi.                                                                                 3:10 to 3:30          -General meeting with team regarding the upcoming works.                                                               3:30 to  4:00          -working on view responses page.                                                               4:00 to 4:15           -Break.                                                       4:15  to 5:45          -continued on responses listing page.   9:00  to 12:00        - Desiging the table for listing.</t>
   </si>
   <si>
     <t>Sheik Fareeth H</t>
@@ -10516,29 +10524,29 @@
 </file>
 
 <file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{30068384-12DE-47D6-BBCA-E055BAD398DB}" name="Table2621016182022242832" displayName="Table2621016182022242832" ref="B9:H19" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{908B1DB8-78D8-42F5-8CBF-7B58FEA062AE}" name="Table262101618202224283234" displayName="Table262101618202224283234" ref="B9:H19" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
   <autoFilter ref="B9:H19" xr:uid="{E9A240DE-1194-474C-BF89-6BCD9A8E6CDB}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F3206353-3602-4878-9C9A-7C40B9BB164C}" name="Resource Name" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{B452D384-A177-4265-8CC5-D9809BCC8BF9}" name="In-progress" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{BBCD43F3-8BA9-4B33-8998-22D0DA25E0F8}" name="Done" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{95C93300-6925-4D9D-8BFD-DF451704C01E}" name="Discarded / Hold" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{52FC73D1-CDC6-4C6D-9836-8BD429F44B3D}" name="Hours Spent - Project" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{2FBB98A1-BCC2-492C-A9CC-2F61DC3BB978}" name="Hours Spent - Non Project" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{D6EE03A5-7AB1-4BB2-B135-D17856E3B216}" name="Comments" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{43267CDA-2000-41A4-A09C-87304607AEA3}" name="Resource Name" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{BD419325-803B-4268-A12E-76D50FCF15DD}" name="In-progress" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{97D4402C-CB2C-493D-9484-2AA7CDF4B5E8}" name="Done" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{E53C0155-55B8-4C5C-8594-C4D413BA8BD6}" name="Discarded / Hold" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{4A5213A3-DF44-49F4-9A71-CB87AA35B8A7}" name="Hours Spent - Project" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{003E4CF5-180C-4117-89B1-DC2B72B3D6CA}" name="Hours Spent - Non Project" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{4FA0C9B6-6BF8-4886-A41C-2FEBB3CF204D}" name="Comments" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{000AB6B3-0207-412D-A260-718914976465}" name="Table3751117192123252933" displayName="Table3751117192123252933" ref="B4:E6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{20284A4A-B5E6-4400-ABFA-FDC1D00C7212}" name="Table375111719212325293335" displayName="Table375111719212325293335" ref="B4:E6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
   <autoFilter ref="B4:E6" xr:uid="{9C7594DF-77AA-4490-AF49-C5C8389AFDB0}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{815B6CE4-634F-4BEF-A3FF-936472880178}" name="Column1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{078417C6-4B24-4FD5-B914-347D7C374AD6}" name="Column2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{F761D6CF-FDF8-4E60-8A84-DAC858233911}" name="Column3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{63AD1974-F6EA-4E94-8F8B-537BB2D78EE2}" name="Column4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{24E9E45B-AD4B-402A-9F47-A4EE22725424}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{C23222EF-801F-4A2B-A41F-3BA035E1A156}" name="Column2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B89C1A74-B9BD-44BC-8B36-A61348536B4D}" name="Column3" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{5A4201D8-E6E3-42F7-BBFC-10E2EC745DA5}" name="Column4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12859,8 +12867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7B8EE2-C09E-4672-919D-0F2EB56C51A0}">
   <dimension ref="A4:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13172,11 +13180,11 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D431D592-0DF9-47E9-858B-9E923A3BA917}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7E5E1D-E354-4FCD-AD92-53A00E511336}">
   <dimension ref="A4:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13396,7 +13404,7 @@
       </c>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="1:8" ht="395.25" customHeight="1">
+    <row r="16" spans="1:8" ht="401.25" customHeight="1">
       <c r="B16" s="19" t="s">
         <v>30</v>
       </c>
@@ -13404,7 +13412,7 @@
         <v>167</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>41</v>
@@ -13419,13 +13427,13 @@
     </row>
     <row r="17" spans="2:8" ht="409.5" customHeight="1">
       <c r="B17" s="19" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D17" s="47" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Updated Timesheet - Deepika
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet  1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet  1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{085D3301-4CA8-42F3-849C-F6E414C911A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3012F2A7-1FB1-43E2-8290-DD42380AEB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="268">
   <si>
     <t>Column1</t>
   </si>
@@ -1195,6 +1195,26 @@
 12.45 pm - 1.30 pm : Break</t>
   </si>
   <si>
+    <t>CSS file corrections, Profile page alignments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+8:45-9:45 - Prepared layout for Cancel Invite
+9:45-10:45- Softskills Session with Savitha(about Problem Solving)
+10:45-11:00 - Break
+11:00-12:00 - Corrected Layout page for Profile      12:00-1:00 - Made alignment corrections in Cancel Invite
+1:00-2:00 - Lunch
+2:00-3:00 - College Project Review
+3:10-3:30 - Team meeting
+3:30-3:50 - Break
+4:00-5:00 - Done Layout for Cancel Drive(Added radio buttons)
+5:00-5:45 - Made Corrections in Profile page
+9:00-11:15 - Merged Cancel Invite,Cancel Drive &amp; Profile with main layout page</t>
+  </si>
+  <si>
+    <t>Prithvi (CEO)</t>
+  </si>
+  <si>
     <t>Have to split the estimated works with team</t>
   </si>
   <si>
@@ -1222,41 +1242,7 @@
     <t>Sheik Fareeth H</t>
   </si>
   <si>
-    <t>Estimation &amp; Prioritize API's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-8.45 to 9.00 : Checking mails
-9.00 to 9.15 : Updating MOM
-9.15 to 9.30 : Surfed how to publish HTML pages
-9.45 to 10.30 : Soft skill session with Savitha.
-10.30 to 11.00 : Break
-11.00 to 12.00 : Identifying unique pages and Operations for Estimation
-12.00 to 1.00 : Listing down the API usage for particular pages for reuse and Estimation
-1.00 to 2.00 : Lunch 
-2.00 to 2.30 : Worked on Estimation
-2.30 to 2.50 : Review Meeting With Rafi
-3.10 to 3.30 : General Team Meating about Progress of team, Team participation, and upcoming works.
-3.30 to 4.00 : Worked on Listing Down API's of Management &amp; Interviewer for estimation.
-4.00 to 4.30 : Break
-4.30 to 6.00 : Completed Verification of API &amp; Operations for all users ( Estimation)
-8.00 to 9.00 : Worked on Most reused API &amp; Operation for Priority.
-</t>
-  </si>
-  <si>
-    <t>Working on UI flow</t>
-  </si>
-  <si>
-    <t>8.45 am - 9.30 am : worked on Login page 
-9.45 am - 10.30 am : Soft skill Session with savitha
-11.00 am - 12.30 pm : worked on register page 
-1.30 pm - 2.30 pm :Worked on Common Layout page
-2.30 pm - 2.50 pm : Review with rafi
-3.10 pm - 3.30 : Team Meeting
-3.30 - 4.00 : Worked on common layout page
-4.30 - 5.45 :Worked on common layout page
-7.00 - 8.00 : completed common layout page
-9.00 - 11.00 : Worked on current drives, home, profile, view response</t>
+    <t>Vinoth (TL)</t>
   </si>
   <si>
     <t xml:space="preserve">Yesterday:                                                                        
@@ -1267,9 +1253,6 @@
 6.30 pm to 8.30 pm : Worked on Admin's Location page  - Back button, add location button.
 8.30 pm to 10.30 pm : Break
 10.30 pm to 12 pm : Verifying and paginating Admin's Location page - Responsiveness
-8.45 am  -  9.00 am : Checking mails
-9.00 am - 11.30 am : Working on Admin's add location - Layout 
-11.30 am to 12.30 : Making changes on Admi's location page - Alignment Problem
 </t>
   </si>
 </sst>
@@ -13210,10 +13193,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7E5E1D-E354-4FCD-AD92-53A00E511336}">
-  <dimension ref="A4:H19"/>
+  <dimension ref="A4:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13353,24 +13336,24 @@
       </c>
       <c r="H11" s="24"/>
     </row>
-    <row r="12" spans="1:8" ht="327.75" customHeight="1">
+    <row r="12" spans="1:8" ht="373.5" customHeight="1">
       <c r="B12" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>160</v>
+        <v>259</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="E12" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="35">
-        <v>4.0999999999999996</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="G12" s="35">
-        <v>1</v>
+        <v>3.3</v>
       </c>
       <c r="H12" s="24"/>
     </row>
@@ -13414,13 +13397,13 @@
     </row>
     <row r="15" spans="1:8" ht="405" customHeight="1">
       <c r="B15" s="19" t="s">
-        <v>27</v>
+        <v>261</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D15" s="44" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
@@ -13441,56 +13424,42 @@
         <v>167</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F16" s="35">
-        <v>3</v>
+        <v>6.15</v>
       </c>
       <c r="G16" s="35">
-        <v>1.1499999999999999</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="H16" s="25"/>
     </row>
-    <row r="17" spans="2:8" ht="409.5" customHeight="1">
+    <row r="17" spans="2:8" ht="401.25" customHeight="1">
       <c r="B17" s="19" t="s">
-        <v>262</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>263</v>
-      </c>
-      <c r="D17" s="47" t="s">
-        <v>264</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="45"/>
+        <v>265</v>
+      </c>
+      <c r="C17" s="35"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="26"/>
-    </row>
-    <row r="18" spans="2:8" ht="291.75" customHeight="1">
+      <c r="H17" s="25"/>
+    </row>
+    <row r="18" spans="2:8" ht="401.25" customHeight="1">
       <c r="B18" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>265</v>
-      </c>
-      <c r="D18" s="44" t="s">
         <v>266</v>
       </c>
+      <c r="C18" s="35"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="35"/>
-      <c r="F18" s="35">
-        <v>9.25</v>
-      </c>
-      <c r="G18" s="35" t="s">
-        <v>217</v>
-      </c>
-      <c r="H18" s="27"/>
-    </row>
-    <row r="19" spans="2:8" ht="208.5" customHeight="1">
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="25"/>
+    </row>
+    <row r="19" spans="2:8" ht="409.5" customHeight="1">
       <c r="B19" s="21" t="s">
         <v>54</v>
       </c>
@@ -13511,6 +13480,8 @@
       </c>
       <c r="H19" s="28"/>
     </row>
+    <row r="20" spans="2:8" ht="291.75" customHeight="1"/>
+    <row r="21" spans="2:8" ht="208.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">

</xml_diff>